<commit_message>
iGate v5.0.19 Release 적용
</commit_message>
<xml_diff>
--- a/Run-Env/iManager/src/main/webapp/template/List_ExceptionLog.xlsx
+++ b/Run-Env/iManager/src/main/webapp/template/List_ExceptionLog.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="21">
   <si>
     <t>에러로그 ID</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -94,6 +94,14 @@
   </si>
   <si>
     <t>에러 코드</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>서비스 ID</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>서비스 ID</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
 </sst>
@@ -514,21 +522,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L11"/>
+  <dimension ref="A1:M11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="I4" sqref="I4:J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="10" width="17.375" customWidth="1"/>
-    <col min="11" max="11" width="42.5" customWidth="1"/>
-    <col min="12" max="12" width="84.375" customWidth="1"/>
+    <col min="1" max="11" width="17.375" customWidth="1"/>
+    <col min="12" max="12" width="42.5" customWidth="1"/>
+    <col min="13" max="13" width="84.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="1:12" s="3" customFormat="1" ht="50.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:13" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="1:13" s="3" customFormat="1" ht="50.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="5" t="s">
         <v>17</v>
       </c>
@@ -542,9 +550,10 @@
       <c r="I2" s="6"/>
       <c r="J2" s="6"/>
       <c r="K2" s="6"/>
-      <c r="L2" s="7"/>
+      <c r="L2" s="6"/>
+      <c r="M2" s="7"/>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>12</v>
       </c>
@@ -561,10 +570,14 @@
         <v>14</v>
       </c>
       <c r="H4" s="1"/>
+      <c r="I4" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="J4" s="1"/>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="B5" s="1"/>
       <c r="C5" s="4" t="s">
@@ -579,8 +592,9 @@
         <v>10</v>
       </c>
       <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>6</v>
       </c>
@@ -609,16 +623,19 @@
         <v>10</v>
       </c>
       <c r="J7" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="K7" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="K7" s="2" t="s">
+      <c r="L7" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="L7" s="2" t="s">
+      <c r="M7" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
@@ -631,8 +648,9 @@
       <c r="J8" s="1"/>
       <c r="K8" s="1"/>
       <c r="L8" s="1"/>
+      <c r="M8" s="1"/>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
@@ -645,8 +663,9 @@
       <c r="J9" s="1"/>
       <c r="K9" s="1"/>
       <c r="L9" s="1"/>
+      <c r="M9" s="1"/>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
@@ -659,8 +678,9 @@
       <c r="J10" s="1"/>
       <c r="K10" s="1"/>
       <c r="L10" s="1"/>
+      <c r="M10" s="1"/>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
@@ -673,10 +693,11 @@
       <c r="J11" s="1"/>
       <c r="K11" s="1"/>
       <c r="L11" s="1"/>
+      <c r="M11" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A2:L2"/>
+    <mergeCell ref="A2:M2"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
iGate v5.0.22 Release 적용
</commit_message>
<xml_diff>
--- a/Run-Env/iManager/src/main/webapp/template/List_ExceptionLog.xlsx
+++ b/Run-Env/iManager/src/main/webapp/template/List_ExceptionLog.xlsx
@@ -3,23 +3,19 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\ESB_workspace\workspace\Git\iGate_v5\Custom\iManager\src\main\webapp\template\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20910" windowHeight="8775"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21240" windowHeight="4155"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet0" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="22">
   <si>
     <t>에러로그 ID</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -102,6 +98,10 @@
   </si>
   <si>
     <t>서비스 ID</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>에러로그 ID</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
 </sst>
@@ -524,7 +524,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H4" sqref="H4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
@@ -590,7 +592,9 @@
         <v>10</v>
       </c>
       <c r="H5" s="1"/>
-      <c r="I5" s="1"/>
+      <c r="I5" s="4" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">

</xml_diff>